<commit_message>
4th, 5th found and not found websites scenario also completed
</commit_message>
<xml_diff>
--- a/src/test/testdata/Accurate_Bucket_ORG_PROV_Phone.xlsx
+++ b/src/test/testdata/Accurate_Bucket_ORG_PROV_Phone.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R3_Report_Automation\src\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87475DF3-7224-4D62-9806-5CCB65E4F31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7B5256-A945-4B1F-B8E9-72E2BA4A6380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2855E3E2-C5F0-4EF0-BC43-ED693B49271B}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <t>No. of R3 Excel Row's to Execute</t>
   </si>
   <si>
-    <t>1</t>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>